<commit_message>
modified:   daily_wl&meteo_data.xlsx 	modified:   data/dam_bathymetry/dam_bathymetry.dbf 	modified:   session_3_geopandas_exercise.ipynb 	modified:   session_4_time_series.ipynb 	modified:   session_5_water_balance.ipynb
</commit_message>
<xml_diff>
--- a/daily_wl&meteo_data.xlsx
+++ b/daily_wl&meteo_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>temperature</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>wl</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>area</t>
   </si>
 </sst>
 </file>
@@ -389,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +414,14 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>41511</v>
       </c>
@@ -425,8 +437,14 @@
       <c r="E2">
         <v>-0.4813327981666672</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1188.982978408122</v>
+      </c>
+      <c r="G2">
+        <v>1309.12227472864</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>41512</v>
       </c>
@@ -442,8 +460,14 @@
       <c r="E3">
         <v>-0.4916947500000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>1175.44415719192</v>
+      </c>
+      <c r="G3">
+        <v>1302.02440134432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>41513</v>
       </c>
@@ -459,8 +483,14 @@
       <c r="E4">
         <v>-0.4984080450000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>1166.708590436828</v>
+      </c>
+      <c r="G4">
+        <v>1297.418220581114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>41514</v>
       </c>
@@ -476,8 +506,14 @@
       <c r="E5">
         <v>-0.5050523225833339</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>1158.090844496391</v>
+      </c>
+      <c r="G5">
+        <v>1292.853549788126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>41515</v>
       </c>
@@ -493,8 +529,14 @@
       <c r="E6">
         <v>-0.5059663823333337</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>1156.907481516007</v>
+      </c>
+      <c r="G6">
+        <v>1292.225130706825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>41516</v>
       </c>
@@ -510,8 +552,14 @@
       <c r="E7">
         <v>-0.5085351710833338</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>1153.584709694915</v>
+      </c>
+      <c r="G7">
+        <v>1290.458495333775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>41517</v>
       </c>
@@ -527,8 +575,14 @@
       <c r="E8">
         <v>-0.515410375</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>1144.712194893297</v>
+      </c>
+      <c r="G8">
+        <v>1285.725974145315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>41518</v>
       </c>
@@ -544,8 +598,14 @@
       <c r="E9">
         <v>-0.5240400157500003</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>1133.618369250074</v>
+      </c>
+      <c r="G9">
+        <v>1279.777112510194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>41519</v>
       </c>
@@ -561,8 +621,14 @@
       <c r="E10">
         <v>-0.5327231916666669</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>1122.50410534907</v>
+      </c>
+      <c r="G10">
+        <v>1273.781642356856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>41520</v>
       </c>
@@ -578,8 +644,14 @@
       <c r="E11">
         <v>-0.5398952166666668</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>1113.360897478052</v>
+      </c>
+      <c r="G11">
+        <v>1268.822264948495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>41521</v>
       </c>
@@ -595,8 +667,14 @@
       <c r="E12">
         <v>-0.5495123574166668</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>1101.153147688985</v>
+      </c>
+      <c r="G12">
+        <v>1262.161765668174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>41522</v>
       </c>
@@ -612,8 +690,14 @@
       <c r="E13">
         <v>-0.5552001065000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>1093.961773122769</v>
+      </c>
+      <c r="G13">
+        <v>1258.217056013558</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>41523</v>
       </c>
@@ -629,8 +713,14 @@
       <c r="E14">
         <v>-0.5588894657500002</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>1089.30846611544</v>
+      </c>
+      <c r="G14">
+        <v>1255.656107130555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>41524</v>
       </c>
@@ -646,8 +736,14 @@
       <c r="E15">
         <v>-0.5655216657500004</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>1080.966017677954</v>
+      </c>
+      <c r="G15">
+        <v>1251.048024104083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>41525</v>
       </c>
@@ -663,8 +759,14 @@
       <c r="E16">
         <v>-0.5725910815000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>1072.10571016804</v>
+      </c>
+      <c r="G16">
+        <v>1246.12996618172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>41526</v>
       </c>
@@ -680,8 +782,14 @@
       <c r="E17">
         <v>-0.5797351315</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>1063.185669755128</v>
+      </c>
+      <c r="G17">
+        <v>1241.153485851195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>41527</v>
       </c>
@@ -697,8 +805,14 @@
       <c r="E18">
         <v>-0.5815806594166668</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>1060.886892141496</v>
+      </c>
+      <c r="G18">
+        <v>1239.866844546268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>41528</v>
       </c>
@@ -714,8 +828,14 @@
       <c r="E19">
         <v>-0.5877324666666666</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>1053.240732939694</v>
+      </c>
+      <c r="G19">
+        <v>1235.574849439349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>41529</v>
       </c>
@@ -731,8 +851,14 @@
       <c r="E20">
         <v>-0.5918493400000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>1048.138026882144</v>
+      </c>
+      <c r="G20">
+        <v>1232.699870829974</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>41530</v>
       </c>
@@ -748,8 +874,14 @@
       <c r="E21">
         <v>-0.5781302065833337</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>1065.186606334921</v>
+      </c>
+      <c r="G21">
+        <v>1242.272031578425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>41531</v>
       </c>
@@ -765,8 +897,14 @@
       <c r="E22">
         <v>-0.5828805111666671</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>1059.269174342304</v>
+      </c>
+      <c r="G22">
+        <v>1238.960368421241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>41532</v>
       </c>
@@ -782,8 +920,14 @@
       <c r="E23">
         <v>-0.5885261790000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>1052.256069268239</v>
+      </c>
+      <c r="G23">
+        <v>1235.020737777558</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>41533</v>
       </c>
@@ -799,8 +943,14 @@
       <c r="E24">
         <v>-0.5926303840833337</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>1047.171241507474</v>
+      </c>
+      <c r="G24">
+        <v>1232.154190068008</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>41534</v>
       </c>
@@ -816,8 +966,14 @@
       <c r="E25">
         <v>-0.5943261384166671</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>1045.073634084376</v>
+      </c>
+      <c r="G25">
+        <v>1230.969171400322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>41535</v>
       </c>
@@ -833,8 +989,14 @@
       <c r="E26">
         <v>-0.5949139674166668</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>1044.346956839151</v>
+      </c>
+      <c r="G26">
+        <v>1230.55830113888</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
         <v>41536</v>
       </c>
@@ -850,8 +1012,14 @@
       <c r="E27">
         <v>-0.598445982166667</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>1039.985579862514</v>
+      </c>
+      <c r="G27">
+        <v>1228.088617767103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>41537</v>
       </c>
@@ -867,8 +1035,14 @@
       <c r="E28">
         <v>-0.602581333416667</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>1034.889929685316</v>
+      </c>
+      <c r="G28">
+        <v>1225.195017026487</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>41538</v>
       </c>
@@ -884,8 +1058,14 @@
       <c r="E29">
         <v>-0.6078654221666665</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>1028.395681203122</v>
+      </c>
+      <c r="G29">
+        <v>1221.49439685293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>41539</v>
       </c>
@@ -901,8 +1081,14 @@
       <c r="E30">
         <v>-0.6142562472500005</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>1020.56664103615</v>
+      </c>
+      <c r="G30">
+        <v>1217.013850215973</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>41540</v>
       </c>
@@ -918,8 +1104,14 @@
       <c r="E31">
         <v>-0.6199725922500002</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>1013.587519732172</v>
+      </c>
+      <c r="G31">
+        <v>1213.001667507444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>41541</v>
       </c>
@@ -935,8 +1127,14 @@
       <c r="E32">
         <v>-0.6278609308333331</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>1003.993418111583</v>
+      </c>
+      <c r="G32">
+        <v>1207.457987959265</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>41542</v>
       </c>
@@ -952,8 +1150,14 @@
       <c r="E33">
         <v>-0.6359318060000004</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>994.2216873814868</v>
+      </c>
+      <c r="G33">
+        <v>1201.777558813651</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>41543</v>
       </c>
@@ -969,8 +1173,14 @@
       <c r="E34">
         <v>-0.6403667750000004</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>988.871277634922</v>
+      </c>
+      <c r="G34">
+        <v>1198.652481567177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>41544</v>
       </c>
@@ -986,8 +1196,14 @@
       <c r="E35">
         <v>-0.6457409951666669</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>982.4060378324644</v>
+      </c>
+      <c r="G35">
+        <v>1194.862065829762</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>41545</v>
       </c>
@@ -1003,8 +1219,14 @@
       <c r="E36">
         <v>-0.6494260490833336</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>977.9844970645275</v>
+      </c>
+      <c r="G36">
+        <v>1192.26078743884</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>41546</v>
       </c>
@@ -1020,8 +1242,14 @@
       <c r="E37">
         <v>-0.6562453621666672</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>969.8272871927287</v>
+      </c>
+      <c r="G37">
+        <v>1187.442241207605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>41547</v>
       </c>
@@ -1037,8 +1265,14 @@
       <c r="E38">
         <v>-0.6620648409166666</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>962.8918133718394</v>
+      </c>
+      <c r="G38">
+        <v>1183.325233510847</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>41548</v>
       </c>
@@ -1054,8 +1288,14 @@
       <c r="E39">
         <v>-0.6680011842916672</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>955.8415696015326</v>
+      </c>
+      <c r="G39">
+        <v>1179.12082926065</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>41549</v>
       </c>
@@ -1071,8 +1311,14 @@
       <c r="E40">
         <v>-0.6724347215000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>950.5923102491031</v>
+      </c>
+      <c r="G40">
+        <v>1175.977659436694</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>41550</v>
       </c>
@@ -1088,8 +1334,14 @@
       <c r="E41">
         <v>-0.6787564481666674</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>943.131468668358</v>
+      </c>
+      <c r="G41">
+        <v>1171.491205705453</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>41551</v>
       </c>
@@ -1105,8 +1357,14 @@
       <c r="E42">
         <v>-0.6850397407500003</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>935.7440406765031</v>
+      </c>
+      <c r="G42">
+        <v>1167.026586467924</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
         <v>41552</v>
       </c>
@@ -1122,8 +1380,14 @@
       <c r="E43">
         <v>-0.6944982359999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>924.6763822762965</v>
+      </c>
+      <c r="G43">
+        <v>1160.295510300243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>41553</v>
       </c>
@@ -1139,8 +1403,14 @@
       <c r="E44">
         <v>-0.7016373669166667</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>916.3649669884915</v>
+      </c>
+      <c r="G44">
+        <v>1155.206732704065</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>41554</v>
       </c>
@@ -1156,8 +1426,14 @@
       <c r="E45">
         <v>-0.7084961324166671</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>908.4143490476893</v>
+      </c>
+      <c r="G45">
+        <v>1150.311053296346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>41555</v>
       </c>
@@ -1173,8 +1449,14 @@
       <c r="E46">
         <v>-0.7174470750000005</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>898.0893797159897</v>
+      </c>
+      <c r="G46">
+        <v>1143.91199015669</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>41556</v>
       </c>
@@ -1190,8 +1472,14 @@
       <c r="E47">
         <v>-0.7267089230833336</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>887.4666670413496</v>
+      </c>
+      <c r="G47">
+        <v>1137.278614428801</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="2">
         <v>41557</v>
       </c>
@@ -1207,8 +1495,14 @@
       <c r="E48">
         <v>-0.7335059783333339</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <v>879.7104552210012</v>
+      </c>
+      <c r="G48">
+        <v>1132.402674663302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>41558</v>
       </c>
@@ -1224,8 +1518,14 @@
       <c r="E49">
         <v>-0.7425789500000008</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <v>869.4095324345225</v>
+      </c>
+      <c r="G49">
+        <v>1125.883628145929</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>41559</v>
       </c>
@@ -1241,8 +1541,14 @@
       <c r="E50">
         <v>-0.7499225720833339</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <v>861.1160071422103</v>
+      </c>
+      <c r="G50">
+        <v>1120.598322180063</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>41560</v>
       </c>
@@ -1258,8 +1564,14 @@
       <c r="E51">
         <v>-0.7586025844166671</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <v>851.3641666846715</v>
+      </c>
+      <c r="G51">
+        <v>1114.340940737251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>41561</v>
       </c>
@@ -1275,8 +1587,14 @@
       <c r="E52">
         <v>-0.7671144000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <v>841.8550685442772</v>
+      </c>
+      <c r="G52">
+        <v>1108.193936483685</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>41562</v>
       </c>
@@ -1292,8 +1610,14 @@
       <c r="E53">
         <v>-0.7748320315000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <v>833.2793902590663</v>
+      </c>
+      <c r="G53">
+        <v>1102.611090811128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>41563</v>
       </c>
@@ -1309,8 +1633,14 @@
       <c r="E54">
         <v>-0.7830374700000003</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <v>824.2100051674004</v>
+      </c>
+      <c r="G54">
+        <v>1096.665515316294</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
         <v>41564</v>
       </c>
@@ -1326,8 +1656,14 @@
       <c r="E55">
         <v>-0.7893747013333335</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <v>817.2397223050752</v>
+      </c>
+      <c r="G55">
+        <v>1092.066626531147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="2">
         <v>41565</v>
       </c>
@@ -1343,8 +1679,14 @@
       <c r="E56">
         <v>-0.7995152555833336</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <v>806.148375511284</v>
+      </c>
+      <c r="G56">
+        <v>1084.69491724609</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="2">
         <v>41566</v>
       </c>
@@ -1360,8 +1702,14 @@
       <c r="E57">
         <v>-0.8094696450833337</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>795.3353397097869</v>
+      </c>
+      <c r="G57">
+        <v>1077.443142386995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="2">
         <v>41567</v>
       </c>
@@ -1377,8 +1725,14 @@
       <c r="E58">
         <v>-0.8192931980000004</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <v>784.7372345883505</v>
+      </c>
+      <c r="G58">
+        <v>1070.271612665216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="2">
         <v>41568</v>
       </c>
@@ -1394,8 +1748,14 @@
       <c r="E59">
         <v>-0.8265830329166671</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <v>776.9195207310263</v>
+      </c>
+      <c r="G59">
+        <v>1064.940045842071</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="2">
         <v>41569</v>
       </c>
@@ -1411,8 +1771,14 @@
       <c r="E60">
         <v>-0.8317364817500005</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <v>771.4170631712277</v>
+      </c>
+      <c r="G60">
+        <v>1061.165937603194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="2">
         <v>41570</v>
       </c>
@@ -1428,8 +1794,14 @@
       <c r="E61">
         <v>-0.838613775</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61">
+        <v>764.1052669340095</v>
+      </c>
+      <c r="G61">
+        <v>1056.122862302097</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="2">
         <v>41571</v>
       </c>
@@ -1445,8 +1817,14 @@
       <c r="E62">
         <v>-0.8462803416666672</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <v>755.9965357178241</v>
+      </c>
+      <c r="G62">
+        <v>1050.49220263259</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="2">
         <v>41572</v>
       </c>
@@ -1462,8 +1840,14 @@
       <c r="E63">
         <v>-0.8555182740833339</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <v>746.2850697711997</v>
+      </c>
+      <c r="G63">
+        <v>1043.695064863226</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="2">
         <v>41573</v>
       </c>
@@ -1479,8 +1863,14 @@
       <c r="E64">
         <v>-0.8646285990833334</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <v>736.7713545244999</v>
+      </c>
+      <c r="G64">
+        <v>1036.978491006107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="2">
         <v>41574</v>
       </c>
@@ -1496,8 +1886,14 @@
       <c r="E65">
         <v>-0.8710815000000004</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <v>730.0710370400648</v>
+      </c>
+      <c r="G65">
+        <v>1032.213063375065</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="2">
         <v>41575</v>
       </c>
@@ -1513,8 +1909,14 @@
       <c r="E66">
         <v>-0.8718789043333334</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <v>729.2452675209138</v>
+      </c>
+      <c r="G66">
+        <v>1031.623721599772</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="2">
         <v>41576</v>
       </c>
@@ -1530,8 +1932,14 @@
       <c r="E67">
         <v>-0.8812097083333338</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67">
+        <v>719.6187125736603</v>
+      </c>
+      <c r="G67">
+        <v>1024.719963614177</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="2">
         <v>41577</v>
       </c>
@@ -1547,8 +1955,14 @@
       <c r="E68">
         <v>-0.8896521416666671</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68">
+        <v>710.9662051818111</v>
+      </c>
+      <c r="G68">
+        <v>1018.461424893149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2">
         <v>41578</v>
       </c>
@@ -1564,8 +1978,14 @@
       <c r="E69">
         <v>-0.9004400583333335</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69">
+        <v>699.9895841454261</v>
+      </c>
+      <c r="G69">
+        <v>1010.447399663549</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="2">
         <v>41579</v>
       </c>
@@ -1581,8 +2001,14 @@
       <c r="E70">
         <v>-0.9104144500000003</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70">
+        <v>689.9205164459847</v>
+      </c>
+      <c r="G70">
+        <v>1003.020986531227</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="2">
         <v>41580</v>
       </c>
@@ -1598,8 +2024,14 @@
       <c r="E71">
         <v>-0.921715166666667</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71">
+        <v>678.60542847938</v>
+      </c>
+      <c r="G71">
+        <v>994.5876194472261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="2">
         <v>41581</v>
       </c>
@@ -1615,8 +2047,14 @@
       <c r="E72">
         <v>-0.9336921740833339</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72">
+        <v>666.7212012088191</v>
+      </c>
+      <c r="G72">
+        <v>985.6270170887689</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="2">
         <v>41582</v>
       </c>
@@ -1632,8 +2070,14 @@
       <c r="E73">
         <v>-0.9445252833333337</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73">
+        <v>656.0679969837217</v>
+      </c>
+      <c r="G73">
+        <v>977.5022695003981</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="2">
         <v>41583</v>
       </c>
@@ -1649,8 +2093,14 @@
       <c r="E74">
         <v>-0.9558851972500002</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74">
+        <v>644.9949142504249</v>
+      </c>
+      <c r="G74">
+        <v>968.9621157311974</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="2">
         <v>41584</v>
       </c>
@@ -1666,8 +2116,14 @@
       <c r="E75">
         <v>-0.9683716095833339</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75">
+        <v>632.9400100268635</v>
+      </c>
+      <c r="G75">
+        <v>959.5511918039604</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="2">
         <v>41585</v>
       </c>
@@ -1683,8 +2139,14 @@
       <c r="E76">
         <v>-0.9777372721666666</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76">
+        <v>623.9780759459215</v>
+      </c>
+      <c r="G76">
+        <v>952.4760148108249</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="2">
         <v>41586</v>
       </c>
@@ -1700,8 +2162,14 @@
       <c r="E77">
         <v>-0.9848839058333336</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77">
+        <v>617.1857662882237</v>
+      </c>
+      <c r="G77">
+        <v>947.0678044321913</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="2">
         <v>41587</v>
       </c>
@@ -1717,8 +2185,14 @@
       <c r="E78">
         <v>-0.9937824639166672</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78">
+        <v>608.7844373149278</v>
+      </c>
+      <c r="G78">
+        <v>940.32254997324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="2">
         <v>41588</v>
       </c>
@@ -1734,8 +2208,14 @@
       <c r="E79">
         <v>-1.00338246575</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79">
+        <v>599.7906709775898</v>
+      </c>
+      <c r="G79">
+        <v>933.0316548062136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="2">
         <v>41589</v>
       </c>
@@ -1751,8 +2231,14 @@
       <c r="E80">
         <v>-1.012240549083333</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <v>591.5563422672756</v>
+      </c>
+      <c r="G80">
+        <v>926.2914939669849</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="2">
         <v>41590</v>
       </c>
@@ -1768,8 +2254,14 @@
       <c r="E81">
         <v>-1.021980465750001</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <v>582.5736948852229</v>
+      </c>
+      <c r="G81">
+        <v>918.8663684690828</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="2">
         <v>41591</v>
       </c>
@@ -1785,8 +2277,14 @@
       <c r="E82">
         <v>-1.029915874083334</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <v>575.3106288821155</v>
+      </c>
+      <c r="G82">
+        <v>912.8061763590008</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="2">
         <v>41592</v>
       </c>
@@ -1802,8 +2300,14 @@
       <c r="E83">
         <v>-1.03986081575</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <v>566.2785786032071</v>
+      </c>
+      <c r="G83">
+        <v>905.1978915894283</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="2">
         <v>41593</v>
       </c>
@@ -1819,8 +2323,14 @@
       <c r="E84">
         <v>-1.05035964075</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <v>556.8284315621086</v>
+      </c>
+      <c r="G84">
+        <v>897.1498576126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="2">
         <v>41594</v>
       </c>
@@ -1836,8 +2346,14 @@
       <c r="E85">
         <v>-1.05861235</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <v>549.4613599060788</v>
+      </c>
+      <c r="G85">
+        <v>890.8122419627967</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="2">
         <v>41595</v>
       </c>
@@ -1853,8 +2369,14 @@
       <c r="E86">
         <v>-1.068265289833334</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <v>540.9128761604936</v>
+      </c>
+      <c r="G86">
+        <v>883.3868195870932</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="2">
         <v>41596</v>
       </c>
@@ -1870,8 +2392,14 @@
       <c r="E87">
         <v>-1.0781332705</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <v>532.2504298992185</v>
+      </c>
+      <c r="G87">
+        <v>875.7822706461966</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="2">
         <v>41597</v>
       </c>
@@ -1887,8 +2415,14 @@
       <c r="E88">
         <v>-1.0892354485</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <v>522.5970772711821</v>
+      </c>
+      <c r="G88">
+        <v>867.2103783743514</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="2">
         <v>41598</v>
       </c>
@@ -1904,8 +2438,14 @@
       <c r="E89">
         <v>-1.10185242475</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <v>511.7456351095011</v>
+      </c>
+      <c r="G89">
+        <v>857.4485610989701</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="2">
         <v>41599</v>
       </c>
@@ -1921,8 +2461,14 @@
       <c r="E90">
         <v>-1.110669725</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <v>504.2373969179578</v>
+      </c>
+      <c r="G90">
+        <v>850.6140449933367</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="2">
         <v>41600</v>
       </c>
@@ -1938,8 +2484,14 @@
       <c r="E91">
         <v>-1.119209432416667</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <v>497.0245767957631</v>
+      </c>
+      <c r="G91">
+        <v>843.9851297977805</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="2">
         <v>41601</v>
       </c>
@@ -1955,8 +2507,14 @@
       <c r="E92">
         <v>-1.125714589833334</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <v>491.5691799685308</v>
+      </c>
+      <c r="G92">
+        <v>838.9293507042304</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="2">
         <v>41602</v>
       </c>
@@ -1972,8 +2530,14 @@
       <c r="E93">
         <v>-1.133795424083334</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93">
+        <v>484.8393635204643</v>
+      </c>
+      <c r="G93">
+        <v>832.6416991193355</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="2">
         <v>41603</v>
       </c>
@@ -1989,8 +2553,14 @@
       <c r="E94">
         <v>-1.144353600166667</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <v>476.1248597848783</v>
+      </c>
+      <c r="G94">
+        <v>824.414645027481</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="2">
         <v>41604</v>
       </c>
@@ -2006,8 +2576,14 @@
       <c r="E95">
         <v>-1.1554524285</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <v>467.0599907487915</v>
+      </c>
+      <c r="G95">
+        <v>815.7524006378677</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="2">
         <v>41605</v>
       </c>
@@ -2023,8 +2599,14 @@
       <c r="E96">
         <v>-1.168003242583334</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96">
+        <v>456.927651618905</v>
+      </c>
+      <c r="G96">
+        <v>805.9405090792048</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="2">
         <v>41606</v>
       </c>
@@ -2040,8 +2622,14 @@
       <c r="E97">
         <v>-1.18100774575</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97">
+        <v>446.5616595820416</v>
+      </c>
+      <c r="G97">
+        <v>795.7565004828799</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="2">
         <v>41607</v>
       </c>
@@ -2057,8 +2645,14 @@
       <c r="E98">
         <v>-1.18744276575</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98">
+        <v>441.4821716660231</v>
+      </c>
+      <c r="G98">
+        <v>790.7109125076831</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" s="2">
         <v>41608</v>
       </c>
@@ -2074,8 +2668,14 @@
       <c r="E99">
         <v>-1.198769758333334</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99">
+        <v>432.6214769955504</v>
+      </c>
+      <c r="G99">
+        <v>781.8201213178528</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" s="2">
         <v>41609</v>
       </c>
@@ -2091,8 +2691,14 @@
       <c r="E100">
         <v>-1.21302772</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100">
+        <v>421.6135141576117</v>
+      </c>
+      <c r="G100">
+        <v>770.6125967977788</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" s="2">
         <v>41610</v>
       </c>
@@ -2108,8 +2714,14 @@
       <c r="E101">
         <v>-1.221868565166667</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101">
+        <v>414.8693138935287</v>
+      </c>
+      <c r="G101">
+        <v>763.6548353151156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="2">
         <v>41611</v>
       </c>
@@ -2125,8 +2737,14 @@
       <c r="E102">
         <v>-1.2327910275</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102">
+        <v>406.6232078979683</v>
+      </c>
+      <c r="G102">
+        <v>755.0506995155957</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" s="2">
         <v>41612</v>
       </c>
@@ -2142,8 +2760,14 @@
       <c r="E103">
         <v>-1.243756912250001</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103">
+        <v>398.4399490889241</v>
+      </c>
+      <c r="G103">
+        <v>746.4040652928935</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="2">
         <v>41613</v>
       </c>
@@ -2159,8 +2783,14 @@
       <c r="E104">
         <v>-1.250324461083334</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104">
+        <v>393.5847884399393</v>
+      </c>
+      <c r="G104">
+        <v>741.2219014326341</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="2">
         <v>41614</v>
       </c>
@@ -2176,8 +2806,14 @@
       <c r="E105">
         <v>-1.258205075</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105">
+        <v>387.8042379229914</v>
+      </c>
+      <c r="G105">
+        <v>735.0003814597179</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="2">
         <v>41615</v>
       </c>
@@ -2193,8 +2829,14 @@
       <c r="E106">
         <v>-1.266546829083334</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106">
+        <v>381.7392589333906</v>
+      </c>
+      <c r="G106">
+        <v>728.4112596636207</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="2">
         <v>41616</v>
       </c>
@@ -2210,8 +2852,14 @@
       <c r="E107">
         <v>-1.281252547583334</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107">
+        <v>371.1819731852331</v>
+      </c>
+      <c r="G107">
+        <v>716.7876007437216</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" s="2">
         <v>41617</v>
       </c>
@@ -2227,8 +2875,14 @@
       <c r="E108">
         <v>-1.291048741833334</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108">
+        <v>364.2445449108384</v>
+      </c>
+      <c r="G108">
+        <v>709.0400306623906</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="2">
         <v>41618</v>
       </c>
@@ -2244,8 +2898,14 @@
       <c r="E109">
         <v>-1.303757449333333</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109">
+        <v>355.3579495885228</v>
+      </c>
+      <c r="G109">
+        <v>698.9849960078913</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" s="2">
         <v>41619</v>
       </c>
@@ -2261,8 +2921,14 @@
       <c r="E110">
         <v>-1.3120475065</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110">
+        <v>349.6300508315032</v>
+      </c>
+      <c r="G110">
+        <v>692.4241968056475</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" s="2">
         <v>41620</v>
       </c>
@@ -2278,8 +2944,14 @@
       <c r="E111">
         <v>-1.320928424083333</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111">
+        <v>343.5542266040791</v>
+      </c>
+      <c r="G111">
+        <v>685.3948366837832</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" s="2">
         <v>41621</v>
       </c>
@@ -2295,8 +2967,14 @@
       <c r="E112">
         <v>-1.327045658333333</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112">
+        <v>339.4054141388258</v>
+      </c>
+      <c r="G112">
+        <v>680.5526826337482</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="2">
         <v>41622</v>
       </c>
@@ -2312,8 +2990,14 @@
       <c r="E113">
         <v>-1.333204766666667</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113">
+        <v>335.2580517113504</v>
+      </c>
+      <c r="G113">
+        <v>675.6773672580345</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" s="2">
         <v>41623</v>
       </c>
@@ -2328,6 +3012,12 @@
       </c>
       <c r="E114">
         <v>-1.344173299999999</v>
+      </c>
+      <c r="F114">
+        <v>327.9462455707715</v>
+      </c>
+      <c r="G114">
+        <v>666.9956662298696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>